<commit_message>
Adding NUnit Test Case for Excel
</commit_message>
<xml_diff>
--- a/NUnitAutomationTestingProgram/SampleTests/Excel/Test Click Xpath.xlsx
+++ b/NUnitAutomationTestingProgram/SampleTests/Excel/Test Click Xpath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DuongCh\Projects\SeleniumFramework\NUnitAutomationTestingProgram\SampleTests\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE50BA-4AD5-4F3A-BA69-671445B64A4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B25D68E-2461-4C97-9F17-51E5CB693AE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8D1508E1-AE38-4628-9F19-71503E8C0CED}"/>
   </bookViews>
@@ -48,13 +48,13 @@
     <t>http://the-internet.herokuapp.com/</t>
   </si>
   <si>
-    <t>//a[contains(text(),'Form Authentication')]</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
     <t>ClickElementByXPath</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Form Authentication')]</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -480,13 +480,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="3"/>
     </row>

</xml_diff>